<commit_message>
try to make interactive plot
</commit_message>
<xml_diff>
--- a/DATA/Meta_analysis_EPP.xlsx
+++ b/DATA/Meta_analysis_EPP.xlsx
@@ -231,9 +231,6 @@
     <t>simultaneous polyandry</t>
   </si>
   <si>
-    <t>Lekking</t>
-  </si>
-  <si>
     <t>Ruff</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>OYCA</t>
+  </si>
+  <si>
+    <t>lekking</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
@@ -798,16 +798,16 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -825,16 +825,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -852,16 +852,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -879,16 +879,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -906,16 +906,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -933,16 +933,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
         <v>97</v>
       </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -960,16 +960,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>69</v>
@@ -1005,10 +1005,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
         <v>81</v>
-      </c>
-      <c r="H9" t="s">
-        <v>82</v>
       </c>
       <c r="I9">
         <v>89</v>
@@ -2118,16 +2118,16 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -2136,10 +2136,10 @@
         <v>4</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" t="s">
         <v>85</v>
-      </c>
-      <c r="H33" t="s">
-        <v>86</v>
       </c>
       <c r="I33">
         <v>66</v>
@@ -2157,16 +2157,16 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
         <v>72</v>
       </c>
-      <c r="C34" t="s">
-        <v>73</v>
-      </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -2175,10 +2175,10 @@
         <v>3</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I34">
         <v>34</v>
@@ -2193,16 +2193,16 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
         <v>75</v>
       </c>
-      <c r="C35" t="s">
-        <v>76</v>
-      </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -2211,10 +2211,10 @@
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" t="s">
         <v>89</v>
-      </c>
-      <c r="H35" t="s">
-        <v>90</v>
       </c>
       <c r="I35">
         <v>47</v>
@@ -2232,16 +2232,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>

</xml_diff>